<commit_message>
new data and started fixing up code, can plot chiral data, adding verdet constant calculations next time I work on it
</commit_message>
<xml_diff>
--- a/FaradayData.xlsx
+++ b/FaradayData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09d1f3cf5ee91424/HaydSwanMeta/JupyterCode/Physics 422/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="263" documentId="13_ncr:1_{35D472D5-3081-4040-8BB2-D05E0E66F0B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABA9E511-8F93-470F-9A81-C5643DDBCAE3}"/>
+  <xr:revisionPtr revIDLastSave="452" documentId="13_ncr:1_{35D472D5-3081-4040-8BB2-D05E0E66F0B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4283A2F2-02DC-428B-9BE3-B5D7777FDA84}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{6EAC14A5-1142-496B-AB7A-69A1B1452233}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="56">
   <si>
     <t>B long (cm)</t>
   </si>
@@ -186,6 +186,30 @@
   </si>
   <si>
     <t>nm</t>
+  </si>
+  <si>
+    <t>err=1/16</t>
+  </si>
+  <si>
+    <t>CHIRAL DATA</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Mass</t>
+  </si>
+  <si>
+    <t>55gram</t>
+  </si>
+  <si>
+    <t>2.5err</t>
+  </si>
+  <si>
+    <t>mL</t>
   </si>
 </sst>
 </file>
@@ -7244,20 +7268,23 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A94FD0F2-3F9D-427A-8005-85FE2D896475}">
-  <dimension ref="A1:N57"/>
+  <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55:K56"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="R60" sqref="R60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
       <c r="B1">
-        <v>7.5</v>
+        <v>5.75</v>
       </c>
       <c r="C1" t="s">
         <v>45</v>
@@ -7272,7 +7299,10 @@
         <v>13</v>
       </c>
       <c r="B2">
-        <v>7.5</v>
+        <v>5.75</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
       </c>
       <c r="G2">
         <v>450</v>
@@ -7284,20 +7314,38 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="B3">
-        <v>18.600000000000001</v>
+        <v>6.9375</v>
       </c>
       <c r="L3" s="1"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>51</v>
+      </c>
+      <c r="B4">
+        <v>82.5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
       </c>
       <c r="L4" s="1"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
       <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -7324,13 +7372,43 @@
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="L7" s="1" t="e">
+      <c r="B7">
+        <v>63</v>
+      </c>
+      <c r="C7">
+        <v>63.5</v>
+      </c>
+      <c r="D7">
+        <v>63.5</v>
+      </c>
+      <c r="E7">
+        <v>64</v>
+      </c>
+      <c r="F7">
+        <v>64</v>
+      </c>
+      <c r="G7">
+        <v>64</v>
+      </c>
+      <c r="H7">
+        <v>63</v>
+      </c>
+      <c r="I7">
+        <v>63</v>
+      </c>
+      <c r="J7">
+        <v>64</v>
+      </c>
+      <c r="K7">
+        <v>62</v>
+      </c>
+      <c r="L7" s="1">
         <f>AVERAGE(B7:K7)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N7" t="e">
+        <v>63.4</v>
+      </c>
+      <c r="N7">
         <f>STDEV(B7:K7)/SQRT(10)</f>
-        <v>#DIV/0!</v>
+        <v>0.20816659994661327</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -7338,11 +7416,11 @@
         <v>10</v>
       </c>
       <c r="L8" s="1" t="e">
-        <f t="shared" ref="L8:L53" si="0">AVERAGE(B8:K8)</f>
+        <f>AVERAGE(B8:K8)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N8" t="e">
-        <f t="shared" ref="N8:N57" si="1">STDEV(B8:K8)/SQRT(10)</f>
+        <f>STDEV(B8:K8)/SQRT(10)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7351,11 +7429,11 @@
         <v>11</v>
       </c>
       <c r="L9" s="1" t="e">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(B9:K9)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N9" t="e">
-        <f t="shared" si="1"/>
+        <f>STDEV(B9:K9)/SQRT(10)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7376,12 +7454,12 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="L10:L53" si="0">AVERAGE(B10:K10)</f>
         <v>0.5</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" t="e">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="N10:N57" si="1">STDEV(B10:K10)/SQRT(10)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -7389,13 +7467,43 @@
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="L11" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N11" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="B11">
+        <v>64.5</v>
+      </c>
+      <c r="C11">
+        <v>66</v>
+      </c>
+      <c r="D11">
+        <v>65.5</v>
+      </c>
+      <c r="E11">
+        <v>64</v>
+      </c>
+      <c r="F11">
+        <v>65</v>
+      </c>
+      <c r="G11">
+        <v>63.5</v>
+      </c>
+      <c r="H11">
+        <v>64.5</v>
+      </c>
+      <c r="I11">
+        <v>63.5</v>
+      </c>
+      <c r="J11">
+        <v>65.5</v>
+      </c>
+      <c r="K11">
+        <v>63</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="0"/>
+        <v>64.5</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>0.31622776601683794</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -7454,16 +7562,43 @@
       <c r="A15" t="s">
         <v>9</v>
       </c>
-      <c r="L15" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M15" t="s">
-        <v>15</v>
-      </c>
-      <c r="N15" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="B15">
+        <v>66</v>
+      </c>
+      <c r="C15">
+        <v>66</v>
+      </c>
+      <c r="D15">
+        <v>65.5</v>
+      </c>
+      <c r="E15">
+        <v>65</v>
+      </c>
+      <c r="F15">
+        <v>64</v>
+      </c>
+      <c r="G15">
+        <v>66</v>
+      </c>
+      <c r="H15">
+        <v>65.5</v>
+      </c>
+      <c r="I15">
+        <v>66.5</v>
+      </c>
+      <c r="J15">
+        <v>65</v>
+      </c>
+      <c r="K15">
+        <v>65</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="0"/>
+        <v>65.45</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="1"/>
+        <v>0.22912878474779197</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -7474,9 +7609,6 @@
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="M16" t="s">
-        <v>16</v>
-      </c>
       <c r="N16" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -7489,9 +7621,6 @@
       <c r="L17" s="1" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
-      </c>
-      <c r="M17" t="s">
-        <v>17</v>
       </c>
       <c r="N17" t="e">
         <f t="shared" si="1"/>
@@ -7528,16 +7657,44 @@
       <c r="A19" t="s">
         <v>9</v>
       </c>
-      <c r="L19" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="N19" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="B19">
+        <v>65.5</v>
+      </c>
+      <c r="C19">
+        <v>65</v>
+      </c>
+      <c r="D19">
+        <v>67</v>
+      </c>
+      <c r="E19">
+        <v>66</v>
+      </c>
+      <c r="F19">
+        <v>67</v>
+      </c>
+      <c r="G19">
+        <v>67</v>
+      </c>
+      <c r="H19">
+        <v>65</v>
+      </c>
+      <c r="I19">
+        <v>66.5</v>
+      </c>
+      <c r="J19">
+        <v>67</v>
+      </c>
+      <c r="K19">
+        <v>65.5</v>
+      </c>
+      <c r="L19" s="1">
+        <f t="shared" si="0"/>
+        <v>66.150000000000006</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19">
+        <f t="shared" si="1"/>
+        <v>0.26925824035672519</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -7547,9 +7704,6 @@
       <c r="L20" s="1" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
-      </c>
-      <c r="M20" t="s">
-        <v>18</v>
       </c>
       <c r="N20" t="e">
         <f t="shared" si="1"/>
@@ -7599,16 +7753,43 @@
       <c r="A23" t="s">
         <v>9</v>
       </c>
-      <c r="L23" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M23" t="s">
-        <v>18</v>
-      </c>
-      <c r="N23" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="B23">
+        <v>66.5</v>
+      </c>
+      <c r="C23">
+        <v>67</v>
+      </c>
+      <c r="D23">
+        <v>68</v>
+      </c>
+      <c r="E23">
+        <v>66</v>
+      </c>
+      <c r="F23">
+        <v>67.5</v>
+      </c>
+      <c r="G23">
+        <v>66.5</v>
+      </c>
+      <c r="H23">
+        <v>68</v>
+      </c>
+      <c r="I23">
+        <v>68.5</v>
+      </c>
+      <c r="J23">
+        <v>67.5</v>
+      </c>
+      <c r="K23">
+        <v>66</v>
+      </c>
+      <c r="L23" s="1">
+        <f t="shared" si="0"/>
+        <v>67.150000000000006</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="1"/>
+        <v>0.27938424357067015</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -7618,9 +7799,6 @@
       <c r="L24" s="1" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
-      </c>
-      <c r="M24" t="s">
-        <v>19</v>
       </c>
       <c r="N24" t="e">
         <f t="shared" si="1"/>
@@ -7670,16 +7848,43 @@
       <c r="A27" t="s">
         <v>9</v>
       </c>
-      <c r="L27" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M27" t="s">
-        <v>20</v>
-      </c>
-      <c r="N27" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="B27">
+        <v>68</v>
+      </c>
+      <c r="C27">
+        <v>69</v>
+      </c>
+      <c r="D27">
+        <v>68</v>
+      </c>
+      <c r="E27">
+        <v>67.5</v>
+      </c>
+      <c r="F27">
+        <v>67.5</v>
+      </c>
+      <c r="G27">
+        <v>67.5</v>
+      </c>
+      <c r="H27">
+        <v>69.5</v>
+      </c>
+      <c r="I27">
+        <v>68</v>
+      </c>
+      <c r="J27">
+        <v>67</v>
+      </c>
+      <c r="K27">
+        <v>69</v>
+      </c>
+      <c r="L27" s="1">
+        <f t="shared" si="0"/>
+        <v>68.099999999999994</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="1"/>
+        <v>0.25603819159562025</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -7689,9 +7894,6 @@
       <c r="L28" s="1" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
-      </c>
-      <c r="M28" t="s">
-        <v>21</v>
       </c>
       <c r="N28" t="e">
         <f t="shared" si="1"/>
@@ -7741,16 +7943,43 @@
       <c r="A31" t="s">
         <v>9</v>
       </c>
-      <c r="L31" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M31" t="s">
-        <v>21</v>
-      </c>
-      <c r="N31" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="B31">
+        <v>68.5</v>
+      </c>
+      <c r="C31">
+        <v>70</v>
+      </c>
+      <c r="D31">
+        <v>69.5</v>
+      </c>
+      <c r="E31">
+        <v>69</v>
+      </c>
+      <c r="F31">
+        <v>70.5</v>
+      </c>
+      <c r="G31">
+        <v>70</v>
+      </c>
+      <c r="H31">
+        <v>68.5</v>
+      </c>
+      <c r="I31">
+        <v>69</v>
+      </c>
+      <c r="J31">
+        <v>69</v>
+      </c>
+      <c r="K31">
+        <v>69</v>
+      </c>
+      <c r="L31" s="1">
+        <f t="shared" si="0"/>
+        <v>69.3</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="1"/>
+        <v>0.21343747458109494</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -7760,9 +7989,6 @@
       <c r="L32" s="1" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
-      </c>
-      <c r="M32" t="s">
-        <v>22</v>
       </c>
       <c r="N32" t="e">
         <f t="shared" si="1"/>
@@ -7812,16 +8038,43 @@
       <c r="A35" t="s">
         <v>9</v>
       </c>
-      <c r="L35" s="1" t="e">
+      <c r="B35">
+        <v>69</v>
+      </c>
+      <c r="C35">
+        <v>69.5</v>
+      </c>
+      <c r="D35">
+        <v>68.5</v>
+      </c>
+      <c r="E35">
+        <v>69</v>
+      </c>
+      <c r="F35">
+        <v>70.5</v>
+      </c>
+      <c r="G35">
+        <v>68</v>
+      </c>
+      <c r="H35">
+        <v>72.5</v>
+      </c>
+      <c r="I35">
+        <v>69</v>
+      </c>
+      <c r="J35">
+        <v>69.5</v>
+      </c>
+      <c r="K35">
+        <v>70</v>
+      </c>
+      <c r="L35" s="1">
         <f>AVERAGE(B35:K35)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M35" t="s">
-        <v>22</v>
-      </c>
-      <c r="N35" t="e">
+        <v>69.55</v>
+      </c>
+      <c r="N35">
         <f>STDEV(B35:K35)/SQRT(10)</f>
-        <v>#DIV/0!</v>
+        <v>0.39756201472921876</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -7831,9 +8084,6 @@
       <c r="L36" s="1" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
-      </c>
-      <c r="M36" t="s">
-        <v>23</v>
       </c>
       <c r="N36" t="e">
         <f t="shared" si="1"/>
@@ -7883,16 +8133,43 @@
       <c r="A39" t="s">
         <v>9</v>
       </c>
-      <c r="L39" s="1" t="e">
+      <c r="B39">
+        <v>71</v>
+      </c>
+      <c r="C39">
+        <v>70.5</v>
+      </c>
+      <c r="D39">
+        <v>71</v>
+      </c>
+      <c r="E39">
+        <v>71.5</v>
+      </c>
+      <c r="F39">
+        <v>71</v>
+      </c>
+      <c r="G39">
+        <v>70</v>
+      </c>
+      <c r="H39">
+        <v>70.5</v>
+      </c>
+      <c r="I39">
+        <v>70.5</v>
+      </c>
+      <c r="J39">
+        <v>72</v>
+      </c>
+      <c r="K39">
+        <v>69.5</v>
+      </c>
+      <c r="L39" s="1">
         <f>AVERAGE(B39:K39)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M39" t="s">
-        <v>23</v>
-      </c>
-      <c r="N39" t="e">
+        <v>70.75</v>
+      </c>
+      <c r="N39">
         <f>STDEV(B39:K39)/SQRT(10)</f>
-        <v>#DIV/0!</v>
+        <v>0.2266911751455907</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
@@ -7902,9 +8179,6 @@
       <c r="L40" s="1" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
-      </c>
-      <c r="M40" t="s">
-        <v>24</v>
       </c>
       <c r="N40" t="e">
         <f t="shared" si="1"/>
@@ -7954,16 +8228,43 @@
       <c r="A43" t="s">
         <v>9</v>
       </c>
-      <c r="L43" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M43" t="s">
-        <v>24</v>
-      </c>
-      <c r="N43" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="B43">
+        <v>71.5</v>
+      </c>
+      <c r="C43">
+        <v>71</v>
+      </c>
+      <c r="D43">
+        <v>71</v>
+      </c>
+      <c r="E43">
+        <v>71.5</v>
+      </c>
+      <c r="F43">
+        <v>73</v>
+      </c>
+      <c r="G43">
+        <v>71</v>
+      </c>
+      <c r="H43">
+        <v>70.5</v>
+      </c>
+      <c r="I43">
+        <v>71.5</v>
+      </c>
+      <c r="J43">
+        <v>71</v>
+      </c>
+      <c r="K43">
+        <v>72</v>
+      </c>
+      <c r="L43" s="1">
+        <f t="shared" si="0"/>
+        <v>71.400000000000006</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="1"/>
+        <v>0.22110831935702666</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -7973,9 +8274,6 @@
       <c r="L44" s="1" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
-      </c>
-      <c r="M44" t="s">
-        <v>25</v>
       </c>
       <c r="N44" t="e">
         <f t="shared" si="1"/>
@@ -8025,16 +8323,43 @@
       <c r="A47" t="s">
         <v>9</v>
       </c>
-      <c r="L47" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M47" t="s">
-        <v>25</v>
-      </c>
-      <c r="N47" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="B47">
+        <v>70.5</v>
+      </c>
+      <c r="C47">
+        <v>70</v>
+      </c>
+      <c r="D47">
+        <v>71.5</v>
+      </c>
+      <c r="E47">
+        <v>72</v>
+      </c>
+      <c r="F47">
+        <v>71.5</v>
+      </c>
+      <c r="G47">
+        <v>71.5</v>
+      </c>
+      <c r="H47">
+        <v>71</v>
+      </c>
+      <c r="I47">
+        <v>70.5</v>
+      </c>
+      <c r="J47">
+        <v>71</v>
+      </c>
+      <c r="K47">
+        <v>71.5</v>
+      </c>
+      <c r="L47" s="1">
+        <f t="shared" si="0"/>
+        <v>71.099999999999994</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="1"/>
+        <v>0.19436506316151</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -8044,9 +8369,6 @@
       <c r="L48" s="1" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
-      </c>
-      <c r="M48" t="s">
-        <v>26</v>
       </c>
       <c r="N48" t="e">
         <f t="shared" si="1"/>
@@ -8096,16 +8418,43 @@
       <c r="A51" t="s">
         <v>9</v>
       </c>
-      <c r="L51" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M51" t="s">
-        <v>27</v>
-      </c>
-      <c r="N51" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+      <c r="B51">
+        <v>71</v>
+      </c>
+      <c r="C51">
+        <v>70</v>
+      </c>
+      <c r="D51">
+        <v>70</v>
+      </c>
+      <c r="E51">
+        <v>71</v>
+      </c>
+      <c r="F51">
+        <v>71.5</v>
+      </c>
+      <c r="G51">
+        <v>71</v>
+      </c>
+      <c r="H51">
+        <v>71</v>
+      </c>
+      <c r="I51">
+        <v>71</v>
+      </c>
+      <c r="J51">
+        <v>70.5</v>
+      </c>
+      <c r="K51">
+        <v>70</v>
+      </c>
+      <c r="L51" s="1">
+        <f t="shared" si="0"/>
+        <v>70.7</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="1"/>
+        <v>0.16996731711975949</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
@@ -8116,9 +8465,7 @@
         <f>AVERAGE(B52:K52)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M52" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="M52" s="2"/>
       <c r="N52" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
@@ -8167,16 +8514,43 @@
       <c r="A55" t="s">
         <v>9</v>
       </c>
-      <c r="L55" s="1" t="e">
+      <c r="B55">
+        <v>70</v>
+      </c>
+      <c r="C55">
+        <v>69.5</v>
+      </c>
+      <c r="D55">
+        <v>70</v>
+      </c>
+      <c r="E55">
+        <v>69</v>
+      </c>
+      <c r="F55">
+        <v>70</v>
+      </c>
+      <c r="G55">
+        <v>69.5</v>
+      </c>
+      <c r="H55">
+        <v>69</v>
+      </c>
+      <c r="I55">
+        <v>69</v>
+      </c>
+      <c r="J55">
+        <v>69.5</v>
+      </c>
+      <c r="K55">
+        <v>70</v>
+      </c>
+      <c r="L55" s="1">
         <f t="shared" ref="L55" si="2">AVERAGE(B55:K55)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M55" t="s">
-        <v>27</v>
-      </c>
-      <c r="N55" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>69.55</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="1"/>
+        <v>0.13844373104863458</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
@@ -8187,9 +8561,7 @@
         <f>AVERAGE(B56:K56)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="M56" s="2" t="s">
-        <v>28</v>
-      </c>
+      <c r="M56" s="2"/>
       <c r="N56" t="e">
         <f>STDEV(B56:K56)/SQRT(10)</f>
         <v>#DIV/0!</v>
@@ -8205,6 +8577,95 @@
       </c>
       <c r="N57" t="e">
         <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" s="1">
+        <v>0</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59">
+        <v>48</v>
+      </c>
+      <c r="C59">
+        <v>47</v>
+      </c>
+      <c r="D59">
+        <v>48</v>
+      </c>
+      <c r="E59">
+        <v>47</v>
+      </c>
+      <c r="F59">
+        <v>47.5</v>
+      </c>
+      <c r="G59">
+        <v>47.5</v>
+      </c>
+      <c r="H59">
+        <v>48</v>
+      </c>
+      <c r="I59">
+        <v>47</v>
+      </c>
+      <c r="J59">
+        <v>47.5</v>
+      </c>
+      <c r="K59">
+        <v>48</v>
+      </c>
+      <c r="L59" s="1">
+        <f>AVERAGE(B59:K59)</f>
+        <v>47.55</v>
+      </c>
+      <c r="N59">
+        <f>STDEV(B59:K59)/SQRT(10)</f>
+        <v>0.13844373104863458</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>10</v>
+      </c>
+      <c r="L60" s="1" t="e">
+        <f t="shared" ref="L60:L61" si="4">AVERAGE(B60:K60)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N60" t="e">
+        <f t="shared" ref="N60:N61" si="5">STDEV(B60:K60)/SQRT(10)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>11</v>
+      </c>
+      <c r="L61" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N61" t="e">
+        <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New chiral data, old chiral data might be botched
</commit_message>
<xml_diff>
--- a/FaradayData.xlsx
+++ b/FaradayData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09d1f3cf5ee91424/HaydSwanMeta/JupyterCode/Physics 422/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="452" documentId="13_ncr:1_{35D472D5-3081-4040-8BB2-D05E0E66F0B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4283A2F2-02DC-428B-9BE3-B5D7777FDA84}"/>
+  <xr:revisionPtr revIDLastSave="652" documentId="13_ncr:1_{35D472D5-3081-4040-8BB2-D05E0E66F0B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55152D77-5D87-4F93-8E63-24767BC759E7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{6EAC14A5-1142-496B-AB7A-69A1B1452233}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="7" xr2:uid="{6EAC14A5-1142-496B-AB7A-69A1B1452233}"/>
   </bookViews>
   <sheets>
     <sheet name="ExpParams" sheetId="3" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Rotation1" sheetId="4" r:id="rId5"/>
     <sheet name="Rotation2" sheetId="5" r:id="rId6"/>
     <sheet name="Rotation3" sheetId="7" r:id="rId7"/>
+    <sheet name="Rotation4" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="58">
   <si>
     <t>B long (cm)</t>
   </si>
@@ -210,6 +211,12 @@
   </si>
   <si>
     <t>mL</t>
+  </si>
+  <si>
+    <t>sample</t>
+  </si>
+  <si>
+    <t>initial pol</t>
   </si>
 </sst>
 </file>
@@ -7270,8 +7277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A94FD0F2-3F9D-427A-8005-85FE2D896475}">
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="R60" sqref="R60"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8672,4 +8679,1421 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44605ADF-DAFE-4903-846E-D4893C533D31}">
+  <dimension ref="A1:N61"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="I64" sqref="I64"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2">
+        <v>5.875</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2">
+        <v>535</v>
+      </c>
+      <c r="H2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2">
+        <v>218.5</v>
+      </c>
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3">
+        <v>6.9375</v>
+      </c>
+      <c r="C3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4">
+        <v>82.5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>102</v>
+      </c>
+      <c r="C7">
+        <v>104</v>
+      </c>
+      <c r="D7">
+        <v>102.5</v>
+      </c>
+      <c r="E7">
+        <v>103</v>
+      </c>
+      <c r="F7">
+        <v>103.5</v>
+      </c>
+      <c r="G7">
+        <v>102.5</v>
+      </c>
+      <c r="H7">
+        <v>103.5</v>
+      </c>
+      <c r="I7">
+        <v>104</v>
+      </c>
+      <c r="J7">
+        <v>103</v>
+      </c>
+      <c r="K7">
+        <v>102.5</v>
+      </c>
+      <c r="L7" s="1">
+        <f>AVERAGE(B7:K7)</f>
+        <v>103.05</v>
+      </c>
+      <c r="N7">
+        <f>STDEV(B7:K7)/SQRT(10)</f>
+        <v>0.21666666666666665</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="1" t="e">
+        <f>AVERAGE(B8:K8)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N8" t="e">
+        <f>STDEV(B8:K8)/SQRT(10)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="1" t="e">
+        <f>AVERAGE(B9:K9)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N9" t="e">
+        <f>STDEV(B9:K9)/SQRT(10)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1">
+        <f t="shared" ref="L10:L53" si="0">AVERAGE(B10:K10)</f>
+        <v>0.5</v>
+      </c>
+      <c r="M10" s="1"/>
+      <c r="N10" t="e">
+        <f t="shared" ref="N10:N57" si="1">STDEV(B10:K10)/SQRT(10)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>103</v>
+      </c>
+      <c r="C11">
+        <v>105</v>
+      </c>
+      <c r="D11">
+        <v>105</v>
+      </c>
+      <c r="E11">
+        <v>104.5</v>
+      </c>
+      <c r="F11">
+        <v>104</v>
+      </c>
+      <c r="G11">
+        <v>105</v>
+      </c>
+      <c r="H11">
+        <v>104</v>
+      </c>
+      <c r="I11">
+        <v>105</v>
+      </c>
+      <c r="J11">
+        <v>103.5</v>
+      </c>
+      <c r="K11">
+        <v>104</v>
+      </c>
+      <c r="L11" s="1">
+        <f t="shared" si="0"/>
+        <v>104.3</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>0.22607766610417557</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="L12" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N12" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L13" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N13" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M14" s="1"/>
+      <c r="N14" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15">
+        <v>104.5</v>
+      </c>
+      <c r="C15">
+        <v>105.5</v>
+      </c>
+      <c r="D15">
+        <v>106</v>
+      </c>
+      <c r="E15">
+        <v>104</v>
+      </c>
+      <c r="F15">
+        <v>104.5</v>
+      </c>
+      <c r="G15">
+        <v>104.5</v>
+      </c>
+      <c r="H15">
+        <v>106</v>
+      </c>
+      <c r="I15">
+        <v>104</v>
+      </c>
+      <c r="J15">
+        <v>104</v>
+      </c>
+      <c r="K15">
+        <v>104</v>
+      </c>
+      <c r="L15" s="1">
+        <f t="shared" si="0"/>
+        <v>104.7</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="1"/>
+        <v>0.26034165586355507</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="L16" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N16" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="L17" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N17" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="M18" s="1"/>
+      <c r="N18" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>104</v>
+      </c>
+      <c r="C19">
+        <v>105</v>
+      </c>
+      <c r="D19">
+        <v>104</v>
+      </c>
+      <c r="E19">
+        <v>104.5</v>
+      </c>
+      <c r="F19">
+        <v>104</v>
+      </c>
+      <c r="G19">
+        <v>105</v>
+      </c>
+      <c r="H19">
+        <v>104</v>
+      </c>
+      <c r="I19">
+        <v>104.5</v>
+      </c>
+      <c r="J19">
+        <v>104</v>
+      </c>
+      <c r="K19">
+        <v>105.5</v>
+      </c>
+      <c r="L19" s="1">
+        <f t="shared" si="0"/>
+        <v>104.45</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19">
+        <f t="shared" si="1"/>
+        <v>0.1740051084818425</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="L20" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N20" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="L21" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N21" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2</v>
+      </c>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1">
+        <f>AVERAGE(B22:K22)</f>
+        <v>2</v>
+      </c>
+      <c r="M22" s="1"/>
+      <c r="N22" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23">
+        <v>105</v>
+      </c>
+      <c r="C23">
+        <v>106</v>
+      </c>
+      <c r="D23">
+        <v>105.5</v>
+      </c>
+      <c r="E23">
+        <v>105</v>
+      </c>
+      <c r="F23">
+        <v>105.5</v>
+      </c>
+      <c r="G23">
+        <v>105</v>
+      </c>
+      <c r="H23">
+        <v>107</v>
+      </c>
+      <c r="I23">
+        <v>105.5</v>
+      </c>
+      <c r="J23">
+        <v>105.5</v>
+      </c>
+      <c r="K23">
+        <v>107</v>
+      </c>
+      <c r="L23" s="1">
+        <f t="shared" si="0"/>
+        <v>105.7</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="1"/>
+        <v>0.23804761428476165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="L24" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N24" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="L25" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N25" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2.4990000000000001</v>
+      </c>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1">
+        <f t="shared" si="0"/>
+        <v>2.4990000000000001</v>
+      </c>
+      <c r="M26" s="1"/>
+      <c r="N26" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27">
+        <v>106</v>
+      </c>
+      <c r="C27">
+        <v>106</v>
+      </c>
+      <c r="D27">
+        <v>106</v>
+      </c>
+      <c r="E27">
+        <v>105.5</v>
+      </c>
+      <c r="F27">
+        <v>105</v>
+      </c>
+      <c r="G27">
+        <v>106</v>
+      </c>
+      <c r="H27">
+        <v>105.5</v>
+      </c>
+      <c r="I27">
+        <v>106</v>
+      </c>
+      <c r="J27">
+        <v>106.5</v>
+      </c>
+      <c r="K27">
+        <v>106</v>
+      </c>
+      <c r="L27" s="1">
+        <f t="shared" si="0"/>
+        <v>105.85</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="1"/>
+        <v>0.13017082793177756</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="L28" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N28" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="L29" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N29" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="1">
+        <v>3</v>
+      </c>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="M30" s="1"/>
+      <c r="N30" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31">
+        <v>106</v>
+      </c>
+      <c r="C31">
+        <v>107</v>
+      </c>
+      <c r="D31">
+        <v>106.5</v>
+      </c>
+      <c r="E31">
+        <v>107</v>
+      </c>
+      <c r="F31">
+        <v>107</v>
+      </c>
+      <c r="G31">
+        <v>106.5</v>
+      </c>
+      <c r="H31">
+        <v>106</v>
+      </c>
+      <c r="I31">
+        <v>107</v>
+      </c>
+      <c r="J31">
+        <v>106</v>
+      </c>
+      <c r="K31">
+        <v>107</v>
+      </c>
+      <c r="L31" s="1">
+        <f t="shared" si="0"/>
+        <v>106.6</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="1"/>
+        <v>0.14529663145135577</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="L32" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N32" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>11</v>
+      </c>
+      <c r="L33" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N33" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="M34" s="1"/>
+      <c r="N34" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B35">
+        <v>106.5</v>
+      </c>
+      <c r="C35">
+        <v>108</v>
+      </c>
+      <c r="D35">
+        <v>107</v>
+      </c>
+      <c r="E35">
+        <v>108</v>
+      </c>
+      <c r="F35">
+        <v>106.5</v>
+      </c>
+      <c r="G35">
+        <v>106.5</v>
+      </c>
+      <c r="H35">
+        <v>106</v>
+      </c>
+      <c r="I35">
+        <v>107</v>
+      </c>
+      <c r="J35">
+        <v>106.5</v>
+      </c>
+      <c r="K35">
+        <v>106</v>
+      </c>
+      <c r="L35" s="1">
+        <f>AVERAGE(B35:K35)</f>
+        <v>106.8</v>
+      </c>
+      <c r="N35">
+        <f>STDEV(B35:K35)/SQRT(10)</f>
+        <v>0.22607766610417557</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="L36" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N36" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>11</v>
+      </c>
+      <c r="L37" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N37" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="1">
+        <v>4</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M38" s="1"/>
+      <c r="N38" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>9</v>
+      </c>
+      <c r="B39">
+        <v>106.5</v>
+      </c>
+      <c r="C39">
+        <v>107</v>
+      </c>
+      <c r="D39">
+        <v>107.5</v>
+      </c>
+      <c r="E39">
+        <v>107</v>
+      </c>
+      <c r="F39">
+        <v>108</v>
+      </c>
+      <c r="G39">
+        <v>107</v>
+      </c>
+      <c r="H39">
+        <v>108</v>
+      </c>
+      <c r="I39">
+        <v>107.5</v>
+      </c>
+      <c r="J39">
+        <v>108</v>
+      </c>
+      <c r="K39">
+        <v>107</v>
+      </c>
+      <c r="L39" s="1">
+        <f>AVERAGE(B39:K39)</f>
+        <v>107.35</v>
+      </c>
+      <c r="N39">
+        <f>STDEV(B39:K39)/SQRT(10)</f>
+        <v>0.16749792701868152</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="L40" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N40" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="L41" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N41" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="M42" s="1"/>
+      <c r="N42" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>9</v>
+      </c>
+      <c r="B43">
+        <v>106</v>
+      </c>
+      <c r="C43">
+        <v>106.5</v>
+      </c>
+      <c r="D43">
+        <v>106</v>
+      </c>
+      <c r="E43">
+        <v>106.5</v>
+      </c>
+      <c r="F43">
+        <v>105</v>
+      </c>
+      <c r="G43">
+        <v>106.5</v>
+      </c>
+      <c r="H43">
+        <v>108</v>
+      </c>
+      <c r="I43">
+        <v>106.5</v>
+      </c>
+      <c r="J43">
+        <v>107</v>
+      </c>
+      <c r="K43">
+        <v>105.5</v>
+      </c>
+      <c r="L43" s="1">
+        <f t="shared" si="0"/>
+        <v>106.35</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="1"/>
+        <v>0.25873624493766706</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>10</v>
+      </c>
+      <c r="L44" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N44" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>11</v>
+      </c>
+      <c r="L45" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N45" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="1">
+        <v>5</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="M46" s="1"/>
+      <c r="N46" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>9</v>
+      </c>
+      <c r="B47">
+        <v>106.5</v>
+      </c>
+      <c r="C47">
+        <v>106</v>
+      </c>
+      <c r="D47">
+        <v>105.5</v>
+      </c>
+      <c r="E47">
+        <v>106</v>
+      </c>
+      <c r="F47">
+        <v>106</v>
+      </c>
+      <c r="G47">
+        <v>107</v>
+      </c>
+      <c r="H47">
+        <v>106</v>
+      </c>
+      <c r="I47">
+        <v>107</v>
+      </c>
+      <c r="J47">
+        <v>108</v>
+      </c>
+      <c r="K47">
+        <v>108</v>
+      </c>
+      <c r="L47" s="1">
+        <f t="shared" si="0"/>
+        <v>106.6</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="1"/>
+        <v>0.27688746209726917</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>10</v>
+      </c>
+      <c r="L48" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N48" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>11</v>
+      </c>
+      <c r="L49" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N49" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1">
+        <f>AVERAGE(B50:K50)</f>
+        <v>5.5</v>
+      </c>
+      <c r="M50" s="1"/>
+      <c r="N50" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51">
+        <v>106</v>
+      </c>
+      <c r="C51">
+        <v>105.5</v>
+      </c>
+      <c r="D51">
+        <v>107</v>
+      </c>
+      <c r="E51">
+        <v>106</v>
+      </c>
+      <c r="F51">
+        <v>105.5</v>
+      </c>
+      <c r="G51">
+        <v>107</v>
+      </c>
+      <c r="H51">
+        <v>107</v>
+      </c>
+      <c r="I51">
+        <v>106</v>
+      </c>
+      <c r="J51">
+        <v>105.5</v>
+      </c>
+      <c r="K51">
+        <v>105</v>
+      </c>
+      <c r="L51" s="1">
+        <f t="shared" si="0"/>
+        <v>106.05</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="1"/>
+        <v>0.22912878474779197</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>10</v>
+      </c>
+      <c r="L52" s="1" t="e">
+        <f>AVERAGE(B52:K52)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M52" s="2"/>
+      <c r="N52" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>11</v>
+      </c>
+      <c r="L53" s="1" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N53" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="1">
+        <v>6</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1">
+        <f>AVERAGE(B54:K54)</f>
+        <v>6</v>
+      </c>
+      <c r="M54" s="1"/>
+      <c r="N54" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55">
+        <v>107</v>
+      </c>
+      <c r="C55">
+        <v>106</v>
+      </c>
+      <c r="D55">
+        <v>106</v>
+      </c>
+      <c r="E55">
+        <v>106</v>
+      </c>
+      <c r="F55">
+        <v>105.5</v>
+      </c>
+      <c r="G55">
+        <v>107.5</v>
+      </c>
+      <c r="H55">
+        <v>106</v>
+      </c>
+      <c r="I55">
+        <v>105.5</v>
+      </c>
+      <c r="J55">
+        <v>107</v>
+      </c>
+      <c r="K55">
+        <v>106</v>
+      </c>
+      <c r="L55" s="1">
+        <f t="shared" ref="L55" si="2">AVERAGE(B55:K55)</f>
+        <v>106.25</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="1"/>
+        <v>0.2140872096444188</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>10</v>
+      </c>
+      <c r="L56" s="1" t="e">
+        <f>AVERAGE(B56:K56)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M56" s="2"/>
+      <c r="N56" t="e">
+        <f>STDEV(B56:K56)/SQRT(10)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>11</v>
+      </c>
+      <c r="L57" s="1" t="e">
+        <f t="shared" ref="L57" si="3">AVERAGE(B57:K57)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N57" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" s="1">
+        <v>0</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59">
+        <v>12</v>
+      </c>
+      <c r="C59">
+        <v>11.5</v>
+      </c>
+      <c r="D59">
+        <v>12</v>
+      </c>
+      <c r="E59">
+        <v>11.5</v>
+      </c>
+      <c r="F59">
+        <v>11.5</v>
+      </c>
+      <c r="G59">
+        <v>12</v>
+      </c>
+      <c r="H59">
+        <v>12</v>
+      </c>
+      <c r="I59">
+        <v>11.5</v>
+      </c>
+      <c r="J59">
+        <v>14</v>
+      </c>
+      <c r="K59">
+        <v>12.5</v>
+      </c>
+      <c r="L59" s="1">
+        <f>AVERAGE(B59:K59)</f>
+        <v>12.05</v>
+      </c>
+      <c r="N59">
+        <f>STDEV(B59:K59)/SQRT(10)</f>
+        <v>0.24094720491334934</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>10</v>
+      </c>
+      <c r="L60" s="1" t="e">
+        <f t="shared" ref="L60:L61" si="4">AVERAGE(B60:K60)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N60" t="e">
+        <f t="shared" ref="N60:N61" si="5">STDEV(B60:K60)/SQRT(10)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>11</v>
+      </c>
+      <c r="L61" s="1" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N61" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fiber data and plots, need to get correct error bars though
</commit_message>
<xml_diff>
--- a/FaradayData.xlsx
+++ b/FaradayData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/09d1f3cf5ee91424/HaydSwanMeta/JupyterCode/Physics 422/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="928" documentId="13_ncr:1_{35D472D5-3081-4040-8BB2-D05E0E66F0B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D1FDEF26-F0CC-48CE-BC96-0953C7DCD880}"/>
+  <xr:revisionPtr revIDLastSave="1131" documentId="13_ncr:1_{35D472D5-3081-4040-8BB2-D05E0E66F0B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12D5E8B9-B631-457B-AEFD-0BEFCB0CA7A2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="9" xr2:uid="{6EAC14A5-1142-496B-AB7A-69A1B1452233}"/>
   </bookViews>
@@ -3078,10 +3078,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8F5640-C57C-42CD-85FC-0F28C76F95E9}">
-  <dimension ref="A1:U57"/>
+  <dimension ref="A1:AA57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3089,7 +3089,7 @@
     <col min="1" max="1" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -3101,7 +3101,7 @@
       </c>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>6</v>
       </c>
       <c r="G2">
-        <v>635</v>
+        <v>635.4</v>
       </c>
       <c r="H2" t="s">
         <v>47</v>
@@ -3119,7 +3119,7 @@
       </c>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -3134,7 +3134,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
         <v>59</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -3155,7 +3155,7 @@
       </c>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -3174,54 +3174,84 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <v>1</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
       <c r="B7">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="D7">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="E7">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F7">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="G7">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="H7">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="I7">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="J7">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="K7">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="L7" s="1">
         <f>AVERAGE(B7:K7)</f>
-        <v>30.7</v>
+        <v>8.4</v>
       </c>
       <c r="N7">
         <f>STDEV(B7:K7)/SQRT(10)</f>
-        <v>1.308519095092703</v>
-      </c>
-      <c r="P7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+        <v>1.013245610238044</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -3234,7 +3264,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -3247,7 +3277,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -3275,51 +3305,81 @@
       <c r="P10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>1</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>1</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>1</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>1</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C11">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="D11">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="E11">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="F11">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="G11">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="H11">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="I11">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="J11">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="K11">
-        <v>37</v>
+        <v>5</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" si="0"/>
-        <v>32.1</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="N11">
         <f t="shared" si="1"/>
-        <v>1.3370780746754372</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+        <v>1.5059142664102023</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -3332,7 +3392,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -3345,7 +3405,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -3370,57 +3430,84 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="O14">
-        <v>0.15</v>
-      </c>
       <c r="P14">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>1</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>1</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>1</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
       <c r="B15">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C15">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="D15">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="E15">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="F15">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="G15">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="H15">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="I15">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="J15">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="K15">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="L15" s="1">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>11.5</v>
       </c>
       <c r="N15">
         <f t="shared" si="1"/>
-        <v>2.1756225162774294</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+        <v>0.83333333333333326</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -3433,7 +3520,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -3446,7 +3533,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -3472,54 +3559,84 @@
         <v>#DIV/0!</v>
       </c>
       <c r="P18">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>1</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>1</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>9</v>
       </c>
       <c r="B19">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C19">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D19">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="E19">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="F19">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="G19">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="H19">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="I19">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="J19">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="K19">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="L19" s="1">
         <f t="shared" si="0"/>
-        <v>23.2</v>
+        <v>12.5</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19">
         <f t="shared" si="1"/>
-        <v>1.2719189352225957</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1.3763881881375051</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -3532,7 +3649,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -3545,7 +3662,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
@@ -3570,21 +3687,84 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P22">
+        <v>5</v>
+      </c>
+      <c r="R22">
+        <v>1</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>1</v>
+      </c>
+      <c r="U22">
+        <v>0</v>
+      </c>
+      <c r="V22">
+        <v>1</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <v>1</v>
+      </c>
+      <c r="Y22">
+        <v>0</v>
+      </c>
+      <c r="Z22">
+        <v>1</v>
+      </c>
+      <c r="AA22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>9</v>
       </c>
-      <c r="L23" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N23" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>12</v>
+      </c>
+      <c r="C23">
+        <v>15</v>
+      </c>
+      <c r="D23">
+        <v>12</v>
+      </c>
+      <c r="E23">
+        <v>15</v>
+      </c>
+      <c r="F23">
+        <v>12</v>
+      </c>
+      <c r="G23">
+        <v>15</v>
+      </c>
+      <c r="H23">
+        <v>12</v>
+      </c>
+      <c r="I23">
+        <v>16</v>
+      </c>
+      <c r="J23">
+        <v>11</v>
+      </c>
+      <c r="K23">
+        <v>16</v>
+      </c>
+      <c r="L23" s="1">
+        <f t="shared" si="0"/>
+        <v>13.6</v>
+      </c>
+      <c r="N23">
+        <f t="shared" si="1"/>
+        <v>0.61824123303304768</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -3597,7 +3777,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>11</v>
       </c>
@@ -3610,7 +3790,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
@@ -3635,21 +3815,84 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P26">
+        <v>6</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>1</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>1</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <v>1</v>
+      </c>
+      <c r="X26">
+        <v>0</v>
+      </c>
+      <c r="Y26">
+        <v>1</v>
+      </c>
+      <c r="Z26">
+        <v>0</v>
+      </c>
+      <c r="AA26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>9</v>
       </c>
-      <c r="L27" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N27" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>19</v>
+      </c>
+      <c r="C27">
+        <v>11</v>
+      </c>
+      <c r="D27">
+        <v>19</v>
+      </c>
+      <c r="E27">
+        <v>11</v>
+      </c>
+      <c r="F27">
+        <v>18</v>
+      </c>
+      <c r="G27">
+        <v>11</v>
+      </c>
+      <c r="H27">
+        <v>19</v>
+      </c>
+      <c r="I27">
+        <v>11</v>
+      </c>
+      <c r="J27">
+        <v>19</v>
+      </c>
+      <c r="K27">
+        <v>11</v>
+      </c>
+      <c r="L27" s="1">
+        <f t="shared" si="0"/>
+        <v>14.9</v>
+      </c>
+      <c r="N27">
+        <f t="shared" si="1"/>
+        <v>1.303414319734477</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -3662,7 +3905,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -3675,7 +3918,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>8</v>
       </c>
@@ -3700,21 +3943,84 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P30">
+        <v>7</v>
+      </c>
+      <c r="R30">
+        <v>0</v>
+      </c>
+      <c r="S30">
+        <v>1</v>
+      </c>
+      <c r="T30">
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <v>1</v>
+      </c>
+      <c r="V30">
+        <v>0</v>
+      </c>
+      <c r="W30">
+        <v>1</v>
+      </c>
+      <c r="X30">
+        <v>0</v>
+      </c>
+      <c r="Y30">
+        <v>1</v>
+      </c>
+      <c r="Z30">
+        <v>0</v>
+      </c>
+      <c r="AA30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>9</v>
       </c>
-      <c r="L31" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N31" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>21</v>
+      </c>
+      <c r="C31">
+        <v>11</v>
+      </c>
+      <c r="D31">
+        <v>21</v>
+      </c>
+      <c r="E31">
+        <v>11</v>
+      </c>
+      <c r="F31">
+        <v>16</v>
+      </c>
+      <c r="G31">
+        <v>15</v>
+      </c>
+      <c r="H31">
+        <v>17</v>
+      </c>
+      <c r="I31">
+        <v>15</v>
+      </c>
+      <c r="J31">
+        <v>17</v>
+      </c>
+      <c r="K31">
+        <v>14</v>
+      </c>
+      <c r="L31" s="1">
+        <f t="shared" si="0"/>
+        <v>15.8</v>
+      </c>
+      <c r="N31">
+        <f t="shared" si="1"/>
+        <v>1.0934146311237811</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -3727,7 +4033,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>11</v>
       </c>
@@ -3740,7 +4046,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
@@ -3765,21 +4071,84 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P34">
+        <v>8</v>
+      </c>
+      <c r="R34">
+        <v>1</v>
+      </c>
+      <c r="S34">
+        <v>0</v>
+      </c>
+      <c r="T34">
+        <v>1</v>
+      </c>
+      <c r="U34">
+        <v>0</v>
+      </c>
+      <c r="V34">
+        <v>1</v>
+      </c>
+      <c r="W34">
+        <v>0</v>
+      </c>
+      <c r="X34">
+        <v>1</v>
+      </c>
+      <c r="Y34">
+        <v>0</v>
+      </c>
+      <c r="Z34">
+        <v>1</v>
+      </c>
+      <c r="AA34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>9</v>
       </c>
-      <c r="L35" s="1" t="e">
+      <c r="B35">
+        <v>14</v>
+      </c>
+      <c r="C35">
+        <v>21</v>
+      </c>
+      <c r="D35">
+        <v>13</v>
+      </c>
+      <c r="E35">
+        <v>21</v>
+      </c>
+      <c r="F35">
+        <v>14</v>
+      </c>
+      <c r="G35">
+        <v>21</v>
+      </c>
+      <c r="H35">
+        <v>13</v>
+      </c>
+      <c r="I35">
+        <v>21</v>
+      </c>
+      <c r="J35">
+        <v>13</v>
+      </c>
+      <c r="K35">
+        <v>21</v>
+      </c>
+      <c r="L35" s="1">
         <f>AVERAGE(B35:K35)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N35" t="e">
+        <v>17.2</v>
+      </c>
+      <c r="N35">
         <f>STDEV(B35:K35)/SQRT(10)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1.2719189352225937</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -3792,20 +4161,17 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>11</v>
       </c>
-      <c r="L37" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
+      <c r="L37" s="1"/>
       <c r="N37" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>8</v>
       </c>
@@ -3830,21 +4196,84 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P38">
+        <v>9</v>
+      </c>
+      <c r="R38">
+        <v>1</v>
+      </c>
+      <c r="S38">
+        <v>0</v>
+      </c>
+      <c r="T38">
+        <v>1</v>
+      </c>
+      <c r="U38">
+        <v>0</v>
+      </c>
+      <c r="V38">
+        <v>1</v>
+      </c>
+      <c r="W38">
+        <v>0</v>
+      </c>
+      <c r="X38">
+        <v>1</v>
+      </c>
+      <c r="Y38">
+        <v>0</v>
+      </c>
+      <c r="Z38">
+        <v>1</v>
+      </c>
+      <c r="AA38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>9</v>
       </c>
-      <c r="L39" s="1" t="e">
+      <c r="B39">
+        <v>13</v>
+      </c>
+      <c r="C39">
+        <v>23</v>
+      </c>
+      <c r="D39">
+        <v>14</v>
+      </c>
+      <c r="E39">
+        <v>23</v>
+      </c>
+      <c r="F39">
+        <v>13</v>
+      </c>
+      <c r="G39">
+        <v>23</v>
+      </c>
+      <c r="H39">
+        <v>13</v>
+      </c>
+      <c r="I39">
+        <v>24</v>
+      </c>
+      <c r="J39">
+        <v>14</v>
+      </c>
+      <c r="K39">
+        <v>23</v>
+      </c>
+      <c r="L39" s="1">
         <f>AVERAGE(B39:K39)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N39" t="e">
+        <v>18.3</v>
+      </c>
+      <c r="N39">
         <f>STDEV(B39:K39)/SQRT(10)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1.640121946685672</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -3857,7 +4286,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -3870,7 +4299,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>8</v>
       </c>
@@ -3895,21 +4324,84 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P42">
+        <v>10</v>
+      </c>
+      <c r="R42">
+        <v>0</v>
+      </c>
+      <c r="S42">
+        <v>1</v>
+      </c>
+      <c r="T42">
+        <v>0</v>
+      </c>
+      <c r="U42">
+        <v>1</v>
+      </c>
+      <c r="V42">
+        <v>0</v>
+      </c>
+      <c r="W42">
+        <v>1</v>
+      </c>
+      <c r="X42">
+        <v>0</v>
+      </c>
+      <c r="Y42">
+        <v>1</v>
+      </c>
+      <c r="Z42">
+        <v>0</v>
+      </c>
+      <c r="AA42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>9</v>
       </c>
-      <c r="L43" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N43" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>21</v>
+      </c>
+      <c r="C43">
+        <v>17</v>
+      </c>
+      <c r="D43">
+        <v>22</v>
+      </c>
+      <c r="E43">
+        <v>17</v>
+      </c>
+      <c r="F43">
+        <v>22</v>
+      </c>
+      <c r="G43">
+        <v>18</v>
+      </c>
+      <c r="H43">
+        <v>21</v>
+      </c>
+      <c r="I43">
+        <v>18</v>
+      </c>
+      <c r="J43">
+        <v>22</v>
+      </c>
+      <c r="K43">
+        <v>18</v>
+      </c>
+      <c r="L43" s="1">
+        <f t="shared" si="0"/>
+        <v>19.600000000000001</v>
+      </c>
+      <c r="N43">
+        <f t="shared" si="1"/>
+        <v>0.68637534273246736</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -3922,7 +4414,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -3935,7 +4427,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>8</v>
       </c>
@@ -3960,21 +4452,84 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P46">
+        <v>11</v>
+      </c>
+      <c r="R46">
+        <v>0</v>
+      </c>
+      <c r="S46">
+        <v>1</v>
+      </c>
+      <c r="T46">
+        <v>0</v>
+      </c>
+      <c r="U46">
+        <v>1</v>
+      </c>
+      <c r="V46">
+        <v>0</v>
+      </c>
+      <c r="W46">
+        <v>1</v>
+      </c>
+      <c r="X46">
+        <v>0</v>
+      </c>
+      <c r="Y46">
+        <v>1</v>
+      </c>
+      <c r="Z46">
+        <v>0</v>
+      </c>
+      <c r="AA46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>9</v>
       </c>
-      <c r="L47" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N47" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>25</v>
+      </c>
+      <c r="C47">
+        <v>17</v>
+      </c>
+      <c r="D47">
+        <v>25</v>
+      </c>
+      <c r="E47">
+        <v>17</v>
+      </c>
+      <c r="F47">
+        <v>25</v>
+      </c>
+      <c r="G47">
+        <v>17</v>
+      </c>
+      <c r="H47">
+        <v>25</v>
+      </c>
+      <c r="I47">
+        <v>17</v>
+      </c>
+      <c r="J47">
+        <v>25</v>
+      </c>
+      <c r="K47">
+        <v>17</v>
+      </c>
+      <c r="L47" s="1">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="N47">
+        <f t="shared" si="1"/>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>10</v>
       </c>
@@ -3987,7 +4542,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>11</v>
       </c>
@@ -4000,7 +4555,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>8</v>
       </c>
@@ -4025,21 +4580,84 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P50">
+        <v>12</v>
+      </c>
+      <c r="R50">
+        <v>1</v>
+      </c>
+      <c r="S50">
+        <v>0</v>
+      </c>
+      <c r="T50">
+        <v>1</v>
+      </c>
+      <c r="U50">
+        <v>0</v>
+      </c>
+      <c r="V50">
+        <v>1</v>
+      </c>
+      <c r="W50">
+        <v>0</v>
+      </c>
+      <c r="X50">
+        <v>1</v>
+      </c>
+      <c r="Y50">
+        <v>0</v>
+      </c>
+      <c r="Z50">
+        <v>1</v>
+      </c>
+      <c r="AA50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>9</v>
       </c>
-      <c r="L51" s="1" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N51" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B51">
+        <v>17</v>
+      </c>
+      <c r="C51">
+        <v>26</v>
+      </c>
+      <c r="D51">
+        <v>17</v>
+      </c>
+      <c r="E51">
+        <v>26</v>
+      </c>
+      <c r="F51">
+        <v>17</v>
+      </c>
+      <c r="G51">
+        <v>27</v>
+      </c>
+      <c r="H51">
+        <v>17</v>
+      </c>
+      <c r="I51">
+        <v>26</v>
+      </c>
+      <c r="J51">
+        <v>16</v>
+      </c>
+      <c r="K51">
+        <v>27</v>
+      </c>
+      <c r="L51" s="1">
+        <f t="shared" si="0"/>
+        <v>21.6</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="1"/>
+        <v>1.6069294390925253</v>
+      </c>
+    </row>
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -4053,7 +4671,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>11</v>
       </c>
@@ -4066,7 +4684,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>8</v>
       </c>
@@ -4085,57 +4703,84 @@
       <c r="L54" s="1"/>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
-      <c r="O54">
-        <v>0.3</v>
-      </c>
       <c r="P54">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="R54">
+        <v>1</v>
+      </c>
+      <c r="S54">
+        <v>0</v>
+      </c>
+      <c r="T54">
+        <v>1</v>
+      </c>
+      <c r="U54">
+        <v>0</v>
+      </c>
+      <c r="V54">
+        <v>1</v>
+      </c>
+      <c r="W54">
+        <v>0</v>
+      </c>
+      <c r="X54">
+        <v>1</v>
+      </c>
+      <c r="Y54">
+        <v>0</v>
+      </c>
+      <c r="Z54">
+        <v>1</v>
+      </c>
+      <c r="AA54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>9</v>
       </c>
       <c r="B55">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C55">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D55">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="E55">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F55">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="G55">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="H55">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="I55">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="J55">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="K55">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="L55" s="1">
         <f>AVERAGE(B55:K55)</f>
-        <v>34.200000000000003</v>
+        <v>22.6</v>
       </c>
       <c r="N55">
         <f>STDEV(B55:K55)/SQRT(10)</f>
-        <v>0.96378881965339736</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0.88443327742810429</v>
+      </c>
+    </row>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>10</v>
       </c>
@@ -4148,7 +4793,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>11</v>
       </c>

</xml_diff>